<commit_message>
Revert "Merge branch 'master' of https://github.com/thimma11/ITP_Schnuppertage"
This reverts commit 8c3b173b08498b513de773cb520a68056e33d32b, reversing
changes made to f75c38c45cd1193242519cba9d6e8f8be6e27635.
</commit_message>
<xml_diff>
--- a/F_Feinplanung/schnittstellenbeschreibung.xlsx
+++ b/F_Feinplanung/schnittstellenbeschreibung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -187,24 +187,6 @@
   </si>
   <si>
     <t>Stundenplan eines Schnuppertags</t>
-  </si>
-  <si>
-    <t>/gegenstand</t>
-  </si>
-  <si>
-    <t>/lehrer</t>
-  </si>
-  <si>
-    <t>/fach</t>
-  </si>
-  <si>
-    <t>/gegenstand/1</t>
-  </si>
-  <si>
-    <t>/lehrer/1</t>
-  </si>
-  <si>
-    <t>/fach/1</t>
   </si>
 </sst>
 </file>
@@ -542,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C41"/>
+  <dimension ref="A2:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,73 +790,25 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C26" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>